<commit_message>
linear equatiosn in newborn outcomes and pregnancy supervisor
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_NewbornOutcomes.xlsx
+++ b/resources/ResourceFile_NewbornOutcomes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>base_incidence_low_birth_weight</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t xml:space="preserve">DUMMY </t>
+  </si>
+  <si>
+    <t>prob_enceph_severity</t>
+  </si>
+  <si>
+    <t>[0.422, 0.338, 0.24]</t>
+  </si>
+  <si>
+    <t>prob_retinopathy_severity</t>
+  </si>
+  <si>
+    <t>[0.4, 0.3, 0.2, 0.1]</t>
   </si>
 </sst>
 </file>
@@ -456,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,7 +528,7 @@
       <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -538,7 +550,7 @@
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -549,7 +561,7 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>1.2E-2</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -558,32 +570,29 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>0.214</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>0.01</v>
+        <v>0.214</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>22</v>
@@ -591,89 +600,111 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B13">
-        <v>0.67</v>
+        <v>0.15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>0.77</v>
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>0.56000000000000005</v>
+        <v>0.67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>0.6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
+        <v>0.77</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B17">
-        <v>0.38</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18">
-        <v>0.27700000000000002</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>20</v>
+        <v>0.6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>0.38</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>0.91800000000000004</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correcting flake8 error and changes to resourcefile
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_NewbornOutcomes.xlsx
+++ b/resources/ResourceFile_NewbornOutcomes.xlsx
@@ -474,7 +474,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,9 +686,6 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
         <v>0.38</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -700,9 +697,6 @@
         <v>12</v>
       </c>
       <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
         <v>0.27700000000000002</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -714,9 +708,6 @@
         <v>13</v>
       </c>
       <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
         <v>0.91800000000000004</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -728,9 +719,6 @@
         <v>38</v>
       </c>
       <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
         <v>0.15</v>
       </c>
     </row>

</xml_diff>